<commit_message>
Modified 08/08/2024 12:01:46 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
@@ -664,7 +664,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -799,7 +799,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda CR-V</t>
+          <t>Honda CR-V2024</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Modified 08/08/2024 12:09:05 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
@@ -664,7 +664,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -799,7 +799,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda CR-V2024</t>
+          <t>Honda CR-V</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Modified 08/08/2024 12:11:54 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
@@ -664,7 +664,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -731,7 +731,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Toyota Yaris</t>
+          <t xml:space="preserve">Toyota Yaris </t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -765,7 +765,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>VINFAST VF8</t>
+          <t xml:space="preserve">VINFAST VF8 </t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -799,7 +799,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda CR-V</t>
+          <t xml:space="preserve">Honda CR-V </t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Modified 08/08/2024 12:16:19 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
@@ -664,7 +664,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -731,7 +731,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Toyota Yaris </t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -765,7 +765,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">VINFAST VF8 </t>
+          <t>VINFAST</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -799,7 +799,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Honda CR-V </t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Modified 08/08/2024 02:41:52 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
@@ -664,7 +664,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -799,7 +799,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Honda 2024</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Modified 08/08/2024 03:11:40 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
@@ -146,7 +146,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6000750" cy="4476750"/>
+    <ext cx="5991225" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -171,7 +171,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6000750" cy="4476750"/>
+    <ext cx="5895975" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -221,7 +221,7 @@
       <row>26</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6000750" cy="4476750"/>
+    <ext cx="5895975" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -246,7 +246,7 @@
       <row>52</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6000750" cy="4476750"/>
+    <ext cx="5895975" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -271,7 +271,7 @@
       <row>52</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6000750" cy="4476750"/>
+    <ext cx="5991225" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -321,7 +321,7 @@
       <row>78</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6000750" cy="4476750"/>
+    <ext cx="6057900" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -346,7 +346,7 @@
       <row>104</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6000750" cy="4476750"/>
+    <ext cx="6096000" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="9" name="Image 9" descr="Picture"/>
@@ -664,7 +664,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="61" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -731,7 +731,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Toyota Yaris &lt;re.Match object; span=(13, 17), match='2020'&gt;</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -765,7 +765,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>VINFAST</t>
+          <t>VINFAST VF8 &lt;re.Match object; span=(12, 16), match='2023'&gt;</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -799,7 +799,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda 2024</t>
+          <t>Honda CR-V &lt;re.Match object; span=(11, 15), match='2024'&gt;</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Modified 08/08/2024 03:20:44 PM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-G) - Color-wise Data & Graphs/Test_cars_combined.xlsx
@@ -146,7 +146,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5991225" cy="4476750"/>
+    <ext cx="6000750" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -171,7 +171,7 @@
       <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5895975" cy="4476750"/>
+    <ext cx="6000750" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -221,7 +221,7 @@
       <row>26</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5895975" cy="4476750"/>
+    <ext cx="6000750" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="4" name="Image 4" descr="Picture"/>
@@ -246,7 +246,7 @@
       <row>52</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5895975" cy="4476750"/>
+    <ext cx="6000750" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="5" name="Image 5" descr="Picture"/>
@@ -271,7 +271,7 @@
       <row>52</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5991225" cy="4476750"/>
+    <ext cx="6000750" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="6" name="Image 6" descr="Picture"/>
@@ -321,7 +321,7 @@
       <row>78</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6057900" cy="4476750"/>
+    <ext cx="6000750" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="8" name="Image 8" descr="Picture"/>
@@ -346,7 +346,7 @@
       <row>104</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6096000" cy="4476750"/>
+    <ext cx="6000750" cy="4476750"/>
     <pic>
       <nvPicPr>
         <cNvPr id="9" name="Image 9" descr="Picture"/>
@@ -664,7 +664,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="61" customWidth="1" min="1" max="1"/>
+    <col width="19" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
@@ -731,7 +731,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Toyota Yaris &lt;re.Match object; span=(13, 17), match='2020'&gt;</t>
+          <t>Toyota Yaris 2020</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -765,7 +765,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>VINFAST VF8 &lt;re.Match object; span=(12, 16), match='2023'&gt;</t>
+          <t>VINFAST VF8 2023</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -799,7 +799,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Honda CR-V &lt;re.Match object; span=(11, 15), match='2024'&gt;</t>
+          <t>Honda CR-V 2024</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>